<commit_message>
Fix song detail. Revert codes
</commit_message>
<xml_diff>
--- a/Document/Release/BUGS.xlsx
+++ b/Document/Release/BUGS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="19560" windowHeight="8340"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="19560" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="57">
   <si>
     <t>Inverted setting for check box in SettingActivity.</t>
   </si>
@@ -182,9 +182,6 @@
     <t>Favorite in listviews star</t>
   </si>
   <si>
-    <t>``````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````````</t>
-  </si>
-  <si>
     <t>Screen Orientation settings</t>
   </si>
   <si>
@@ -198,6 +195,9 @@
   </si>
   <si>
     <t>FavoriteFragment</t>
+  </si>
+  <si>
+    <t>Search bar focus white background</t>
   </si>
 </sst>
 </file>
@@ -588,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,10 +792,10 @@
         <v>21</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>7</v>
@@ -896,7 +896,7 @@
         <v>22</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>23</v>
@@ -910,10 +910,10 @@
         <v>22</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>7</v>
@@ -1017,9 +1017,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>51</v>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: setting activity. auto update message splash screen. Empty Views. Network timeout. Change developer mode
</commit_message>
<xml_diff>
--- a/Document/Release/BUGS.xlsx
+++ b/Document/Release/BUGS.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="58">
   <si>
     <t>Inverted setting for check box in SettingActivity.</t>
   </si>
@@ -182,9 +182,6 @@
     <t>Favorite in listviews star</t>
   </si>
   <si>
-    <t>Screen Orientation settings</t>
-  </si>
-  <si>
     <t>Media player error notification more detail</t>
   </si>
   <si>
@@ -198,6 +195,12 @@
   </si>
   <si>
     <t>Search bar focus white background</t>
+  </si>
+  <si>
+    <t>Logout &gt; System exit</t>
+  </si>
+  <si>
+    <t>Screen Orientation keep state</t>
   </si>
 </sst>
 </file>
@@ -220,7 +223,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,6 +239,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -267,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -279,6 +288,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -588,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,40 +644,35 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    </row>
+    <row r="3" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="E3" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:7" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -740,17 +750,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="3" t="s">
+    <row r="9" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -768,7 +778,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
@@ -778,11 +788,9 @@
       <c r="C11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="4"/>
       <c r="G11" s="4" t="s">
         <v>38</v>
       </c>
@@ -792,139 +800,139 @@
         <v>21</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="E12" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="C13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="1:7" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="4" t="s">
+      <c r="A14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    </row>
+    <row r="16" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="E18" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B19" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C19" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="E19" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C20" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="D20" s="4"/>
+      <c r="E20" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="B21" s="3" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>23</v>
@@ -933,107 +941,127 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="E28" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>15</v>
+      <c r="E29" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G17">
-    <sortState ref="A2:G27">
+    <sortState ref="A2:G29">
       <sortCondition ref="A1:A17"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Add CustomFragment for Performance with Sliding Menu
</commit_message>
<xml_diff>
--- a/Document/Release/BUGS.xlsx
+++ b/Document/Release/BUGS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="19560" windowHeight="8340"/>
+    <workbookView xWindow="4650" yWindow="0" windowWidth="19560" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -605,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update bug tracking document
</commit_message>
<xml_diff>
--- a/Document/Release/BUGS.xlsx
+++ b/Document/Release/BUGS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="0" windowWidth="19560" windowHeight="8340"/>
+    <workbookView xWindow="5580" yWindow="0" windowWidth="19560" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,9 +47,6 @@
     <t>Cancel Auto Update no repeat. (HaiNNT)</t>
   </si>
   <si>
-    <t>Song Detail Fragment: minize? (HaiNNT)</t>
-  </si>
-  <si>
     <t>HaiNNT</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>Add playlist button</t>
   </si>
   <si>
-    <t>No more related song: notif user. (HaiNNT)</t>
-  </si>
-  <si>
     <t>MainActivity</t>
   </si>
   <si>
@@ -201,6 +195,12 @@
   </si>
   <si>
     <t>Screen Orientation keep state</t>
+  </si>
+  <si>
+    <t>Song Detail Fragment: minize?</t>
+  </si>
+  <si>
+    <t>No more related song: notif user.</t>
   </si>
 </sst>
 </file>
@@ -605,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,441 +622,438 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="E3" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="4" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
+      <c r="A14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>7</v>
+    <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update bug tracking process...
</commit_message>
<xml_diff>
--- a/Document/Release/BUGS.xlsx
+++ b/Document/Release/BUGS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="0" windowWidth="19560" windowHeight="8340"/>
+    <workbookView xWindow="6510" yWindow="0" windowWidth="19560" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="64">
   <si>
     <t>Inverted setting for check box in SettingActivity.</t>
   </si>
@@ -182,9 +182,6 @@
     <t>MediaPlayer</t>
   </si>
   <si>
-    <t>SQLite LIKE query with utf-8</t>
-  </si>
-  <si>
     <t>FavoriteFragment</t>
   </si>
   <si>
@@ -201,6 +198,27 @@
   </si>
   <si>
     <t>No more related song: notif user.</t>
+  </si>
+  <si>
+    <t>Empty playlist add "Add playlist" button</t>
+  </si>
+  <si>
+    <t>PlaylistManager</t>
+  </si>
+  <si>
+    <t>Duplicate song list Favorite</t>
+  </si>
+  <si>
+    <t>Cancel synching playlist.</t>
+  </si>
+  <si>
+    <t>Don't hide button of related songs</t>
+  </si>
+  <si>
+    <t>Empty song list adapter</t>
+  </si>
+  <si>
+    <t>SQLite LIKE query with utf-8 &gt; ORDER BY TITLE_ASCII</t>
   </si>
 </sst>
 </file>
@@ -603,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,10 +818,10 @@
         <v>19</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>6</v>
@@ -814,7 +832,7 @@
         <v>19</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>12</v>
@@ -828,7 +846,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>37</v>
@@ -838,31 +856,34 @@
       </c>
     </row>
     <row r="15" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="A15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -870,13 +891,13 @@
         <v>20</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -884,10 +905,10 @@
         <v>20</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>6</v>
@@ -898,10 +919,10 @@
         <v>20</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>6</v>
@@ -912,14 +933,14 @@
         <v>20</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -929,38 +950,41 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>6</v>
@@ -968,13 +992,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>6</v>
@@ -982,13 +1006,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>6</v>
@@ -996,13 +1020,13 @@
     </row>
     <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3" t="s">
@@ -1012,31 +1036,28 @@
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
+      <c r="B27" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>6</v>
@@ -1047,18 +1068,91 @@
         <v>23</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E33" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G17">
-    <sortState ref="A2:G29">
+    <sortState ref="A2:G34">
       <sortCondition ref="A1:A17"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Fix search query order ABC. Update bug tracking document
</commit_message>
<xml_diff>
--- a/Document/Release/BUGS.xlsx
+++ b/Document/Release/BUGS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6510" yWindow="0" windowWidth="19560" windowHeight="8340"/>
+    <workbookView xWindow="8370" yWindow="0" windowWidth="19560" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -241,7 +241,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,12 +257,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -294,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -306,9 +300,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -623,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,20 +666,20 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -768,17 +759,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="5" t="s">
+    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -813,17 +804,17 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="3" t="s">
+    <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="4" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix chord view position buttons
</commit_message>
<xml_diff>
--- a/Document/Release/BUGS.xlsx
+++ b/Document/Release/BUGS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8370" yWindow="0" windowWidth="19560" windowHeight="8340"/>
+    <workbookView xWindow="9300" yWindow="0" windowWidth="19560" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -241,7 +241,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,6 +257,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -302,7 +308,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -615,7 +621,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,20 +672,20 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1099,45 +1105,45 @@
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="E32" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="E33" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="4" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix nav drawer playlist add btn, full song screen auto scroll first time, dont hide show more related songs.
</commit_message>
<xml_diff>
--- a/Document/Release/BUGS.xlsx
+++ b/Document/Release/BUGS.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="65">
   <si>
     <t>Inverted setting for check box in SettingActivity.</t>
   </si>
@@ -219,6 +219,9 @@
   </si>
   <si>
     <t>SQLite LIKE query with utf-8 &gt; ORDER BY TITLE_ASCII</t>
+  </si>
+  <si>
+    <t>Avatar png icon black</t>
   </si>
 </sst>
 </file>
@@ -618,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,17 +1004,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1034,69 +1037,75 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="D28" s="3"/>
       <c r="E28" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>8</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="D30" s="3"/>
       <c r="E30" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
@@ -1106,50 +1115,73 @@
       <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C33" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E32" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D33" s="5"/>
+      <c r="E33" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B34" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C35" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E34" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G17">
-    <sortState ref="A2:G34">
+    <sortState ref="A2:G35">
       <sortCondition ref="A1:A17"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Fix empty list view. Fix mp3 dialog message no connection
</commit_message>
<xml_diff>
--- a/Document/Release/BUGS.xlsx
+++ b/Document/Release/BUGS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9300" yWindow="0" windowWidth="19560" windowHeight="8340"/>
+    <workbookView xWindow="10230" yWindow="0" windowWidth="19560" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="67">
   <si>
     <t>Inverted setting for check box in SettingActivity.</t>
   </si>
@@ -222,6 +222,23 @@
   </si>
   <si>
     <t>Avatar png icon black</t>
+  </si>
+  <si>
+    <t>java.lang.IllegalStateException: The content of the adapter has changed but ListView did not receive a notification. Make sure the content of your adapter is not modified from a background thread, but only from the UI thread. [in ListView(2131296325, class com.hqt.hac.helper.widget.InfinityListView) with Adapter(class android.widget.HeaderViewListAdapter)]
+at android.widget.ListView.layoutChildren(ListView.java:1585)
+            at android.widget.AbsListView$CheckForTap.run(AbsListView.java:3006)
+            at android.os.Handler.handleCallback(Handler.java:730)
+            at android.os.Handler.dispatchMessage(Handler.java:92)
+            at android.os.Looper.loop(Looper.java:213)
+            at android.app.ActivityThread.main(ActivityThread.java:5225)
+            at java.lang.reflect.Method.invokeNative(Native Method)
+            at java.lang.reflect.Method.invoke(Method.java:525)
+            at com.android.internal.os.ZygoteInit$MethodAndArgsCaller.run(ZygoteInit.java:741)
+            at com.android.internal.os.ZygoteInit.main(ZygoteInit.java:557)
+            at dalvik.system.NativeStart.main(Native Method)</t>
+  </si>
+  <si>
+    <t>Search for "ka", select Karic, do a very fast up and down scroll</t>
   </si>
 </sst>
 </file>
@@ -621,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,32 +889,37 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>6</v>
-      </c>
+    <row r="16" spans="1:7" s="4" customFormat="1" ht="240" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -905,13 +927,13 @@
         <v>20</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -919,10 +941,10 @@
         <v>20</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>6</v>
@@ -933,10 +955,10 @@
         <v>20</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4" t="s">
@@ -950,13 +972,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -964,148 +986,152 @@
         <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="B23" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="D25" s="3"/>
+      <c r="E25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="E26" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B27" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C27" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D28" s="3"/>
-      <c r="E28" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-    </row>
-    <row r="30" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
@@ -1119,10 +1145,10 @@
         <v>23</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
@@ -1132,45 +1158,45 @@
       <c r="G32" s="4"/>
     </row>
     <row r="33" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C34" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-    </row>
-    <row r="34" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4" t="s">
@@ -1179,9 +1205,26 @@
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
     </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G17">
-    <sortState ref="A2:G35">
+    <sortState ref="A2:G36">
       <sortCondition ref="A1:A17"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Merge. Update bug tracking.
</commit_message>
<xml_diff>
--- a/Document/Release/BUGS.xlsx
+++ b/Document/Release/BUGS.xlsx
@@ -640,7 +640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -873,21 +873,18 @@
       </c>
     </row>
     <row r="15" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="A15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
+      <c r="E15" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="16" spans="1:7" s="4" customFormat="1" ht="240" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -1015,17 +1012,17 @@
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1092,17 +1089,17 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="5" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix design for old androids. Fix SplashScreen
</commit_message>
<xml_diff>
--- a/Document/Release/BUGS.xlsx
+++ b/Document/Release/BUGS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10230" yWindow="0" windowWidth="19560" windowHeight="8340"/>
+    <workbookView xWindow="11160" yWindow="0" windowWidth="19560" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="68">
   <si>
     <t>Inverted setting for check box in SettingActivity.</t>
   </si>
@@ -239,6 +239,9 @@
   </si>
   <si>
     <t>Search for "ka", select Karic, do a very fast up and down scroll</t>
+  </si>
+  <si>
+    <t>Playlist highlight seleted item</t>
   </si>
 </sst>
 </file>
@@ -314,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -329,6 +332,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -638,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,17 +878,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="4" t="s">
+    <row r="15" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1218,6 +1224,17 @@
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G17">

</xml_diff>

<commit_message>
Fix inf listview duplicate done
</commit_message>
<xml_diff>
--- a/Document/Release/BUGS.xlsx
+++ b/Document/Release/BUGS.xlsx
@@ -646,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,17 +850,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="3" t="s">
+    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="6" t="s">
         <v>13</v>
       </c>
     </row>
@@ -878,17 +878,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="6" t="s">
+    <row r="15" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="4" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix navigation drawer selectable
</commit_message>
<xml_diff>
--- a/Document/Release/BUGS.xlsx
+++ b/Document/Release/BUGS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11160" yWindow="0" windowWidth="19560" windowHeight="8340"/>
+    <workbookView xWindow="12090" yWindow="0" windowWidth="19560" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -646,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,21 +1033,18 @@
       </c>
     </row>
     <row r="25" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
+      <c r="E25" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
@@ -1096,25 +1093,26 @@
       <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="A29" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>21</v>
@@ -1127,31 +1125,31 @@
       <c r="G30" s="5"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
+      <c r="B31" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
     </row>
     <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
@@ -1165,58 +1163,55 @@
         <v>23</v>
       </c>
       <c r="B33" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C34" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E33" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+      <c r="E34" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B35" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C35" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4" t="s">
@@ -1226,19 +1221,25 @@
       <c r="G36" s="4"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="A37" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G17">
-    <sortState ref="A2:G36">
+    <sortState ref="A2:G37">
       <sortCondition ref="A1:A17"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Update InfListVew, fix design
</commit_message>
<xml_diff>
--- a/Document/Release/BUGS.xlsx
+++ b/Document/Release/BUGS.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$16</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="68">
   <si>
     <t>Inverted setting for check box in SettingActivity.</t>
   </si>
@@ -224,24 +224,13 @@
     <t>Avatar png icon black</t>
   </si>
   <si>
-    <t>java.lang.IllegalStateException: The content of the adapter has changed but ListView did not receive a notification. Make sure the content of your adapter is not modified from a background thread, but only from the UI thread. [in ListView(2131296325, class com.hqt.hac.helper.widget.InfinityListView) with Adapter(class android.widget.HeaderViewListAdapter)]
-at android.widget.ListView.layoutChildren(ListView.java:1585)
-            at android.widget.AbsListView$CheckForTap.run(AbsListView.java:3006)
-            at android.os.Handler.handleCallback(Handler.java:730)
-            at android.os.Handler.dispatchMessage(Handler.java:92)
-            at android.os.Looper.loop(Looper.java:213)
-            at android.app.ActivityThread.main(ActivityThread.java:5225)
-            at java.lang.reflect.Method.invokeNative(Native Method)
-            at java.lang.reflect.Method.invoke(Method.java:525)
-            at com.android.internal.os.ZygoteInit$MethodAndArgsCaller.run(ZygoteInit.java:741)
-            at com.android.internal.os.ZygoteInit.main(ZygoteInit.java:557)
-            at dalvik.system.NativeStart.main(Native Method)</t>
-  </si>
-  <si>
-    <t>Search for "ka", select Karic, do a very fast up and down scroll</t>
-  </si>
-  <si>
     <t>Playlist highlight seleted item</t>
+  </si>
+  <si>
+    <t>Chord view contact bar for "C, D, E, F"</t>
+  </si>
+  <si>
+    <t>Search by chord not working after update inf listview</t>
   </si>
 </sst>
 </file>
@@ -345,7 +334,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9"/>
+          <bgColor rgb="FFFF7171"/>
         </patternFill>
       </fill>
     </dxf>
@@ -359,7 +348,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF7171"/>
+          <bgColor theme="9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -644,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,37 +881,32 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="4" customFormat="1" ht="240" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+    <row r="16" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="17" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -930,103 +914,103 @@
         <v>20</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E18" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-    </row>
-    <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="4"/>
+        <v>50</v>
+      </c>
       <c r="E23" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>6</v>
@@ -1037,82 +1021,81 @@
         <v>20</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>7</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D26" s="4"/>
       <c r="E26" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-    </row>
-    <row r="28" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="3" t="s">
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-    </row>
-    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C29" s="3" t="s">
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-    </row>
-    <row r="30" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>21</v>
@@ -1124,94 +1107,94 @@
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-    </row>
-    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D32" s="4"/>
+        <v>8</v>
+      </c>
       <c r="E32" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
     </row>
     <row r="33" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C34" s="4" t="s">
+      <c r="B34" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E34" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C35" s="5" t="s">
+      <c r="B35" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4" t="s">
@@ -1221,37 +1204,42 @@
       <c r="G36" s="4"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
+      <c r="A37" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G17">
+  <autoFilter ref="A1:G16">
     <sortState ref="A2:G37">
       <sortCondition ref="A1:A17"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>"BUG"</formula>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"UPDATE"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"FIX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"UPDATE"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"BUG"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix chord view SearchIndexer. Update bug tracking document
</commit_message>
<xml_diff>
--- a/Document/Release/BUGS.xlsx
+++ b/Document/Release/BUGS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12090" yWindow="0" windowWidth="19560" windowHeight="8340"/>
+    <workbookView xWindow="13020" yWindow="0" windowWidth="19560" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -636,7 +636,7 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1203,14 +1203,14 @@
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B37" s="3" t="s">
+    <row r="37" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="4" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Backup before refactor pakages
</commit_message>
<xml_diff>
--- a/Document/Release/BUGS.xlsx
+++ b/Document/Release/BUGS.xlsx
@@ -635,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,107 +1074,99 @@
       </c>
     </row>
     <row r="29" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B31" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C31" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="E31" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B32" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C32" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-    </row>
-    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-    </row>
-    <row r="32" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
     </row>
     <row r="33" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
+      <c r="B34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>7</v>
@@ -1187,48 +1179,54 @@
       <c r="G35" s="4"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
+      <c r="B36" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
     </row>
     <row r="37" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>42</v>
+        <v>7</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>15</v>
+        <v>58</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G16">
-    <sortState ref="A2:G37">
-      <sortCondition ref="A1:A17"/>
+    <sortState ref="A2:G38">
+      <sortCondition ref="A1:A16"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="A1:A1048576">

</xml_diff>